<commit_message>
updating business process sheet and adding a new BSCS interface document
git-tfs-id: [http://developmentvlan:8585/tfs/vanrise.collection]$/;C55339
</commit_message>
<xml_diff>
--- a/SOM/Documents/SOM/Business Processes.xlsx
+++ b/SOM/Documents/SOM/Business Processes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="78">
   <si>
     <t>Name</t>
   </si>
@@ -62,30 +62,15 @@
     <t>S2C3202</t>
   </si>
   <si>
-    <t>Could not find the use case details in HLD</t>
-  </si>
-  <si>
-    <t>S2C3139</t>
-  </si>
-  <si>
     <t>S2C3138</t>
   </si>
   <si>
-    <t>L2S3129</t>
-  </si>
-  <si>
-    <t>S2C3120 is activate and L2S3129 is create which one to use?</t>
-  </si>
-  <si>
     <t>ST_AddOtherCharges</t>
   </si>
   <si>
     <t>L2S3201</t>
   </si>
   <si>
-    <t>is it correct? The use case for this story</t>
-  </si>
-  <si>
     <t>ST_UpdateContractAddress</t>
   </si>
   <si>
@@ -104,9 +89,6 @@
     <t>S2C3151</t>
   </si>
   <si>
-    <t>Is it correct? The use case for this story - no diagram is found</t>
-  </si>
-  <si>
     <t>LOB</t>
   </si>
   <si>
@@ -228,13 +210,61 @@
   </si>
   <si>
     <t>ADSL</t>
+  </si>
+  <si>
+    <t>S2C3122 - S2C3125</t>
+  </si>
+  <si>
+    <t>S2C3125 CRM and S2C3122 OM Logic</t>
+  </si>
+  <si>
+    <t>Only One call and make it a request on CRM</t>
+  </si>
+  <si>
+    <t>S2C3128 CRM and S2C3139 OM Logic</t>
+  </si>
+  <si>
+    <t>S2C3128 - S2C3139</t>
+  </si>
+  <si>
+    <t>Need web service from BSCS</t>
+  </si>
+  <si>
+    <t>L2S3128</t>
+  </si>
+  <si>
+    <t>L2S3128 - S2C3119</t>
+  </si>
+  <si>
+    <t>L2S3128 CRM and S2C3119 OM Logic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L2S3128 create secondary number list </t>
+  </si>
+  <si>
+    <t>L2S3129 - S2C3120</t>
+  </si>
+  <si>
+    <t>L2S3129 CRM and S2C3120 OM</t>
+  </si>
+  <si>
+    <t>Missing in HLD</t>
+  </si>
+  <si>
+    <t>Might be deactivate service</t>
+  </si>
+  <si>
+    <t>S2C3153</t>
+  </si>
+  <si>
+    <t>Does not contain a diagram</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,8 +279,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -260,6 +297,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -276,15 +325,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -568,14 +620,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
     <col min="5" max="5" width="24.140625" customWidth="1"/>
     <col min="6" max="6" width="45.85546875" style="1" customWidth="1"/>
@@ -583,7 +635,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -602,13 +654,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>28</v>
+      <c r="A2" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D2">
@@ -616,11 +668,11 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+      <c r="A3" s="3"/>
       <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D3">
@@ -628,11 +680,11 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="3"/>
       <c r="B4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D4">
@@ -640,23 +692,26 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="3"/>
       <c r="B5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
+        <v>26</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="D5">
         <v>6525</v>
       </c>
+      <c r="F5" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="3"/>
       <c r="B6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D6">
@@ -664,125 +719,146 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="3"/>
       <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D7">
         <v>6702</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="3"/>
       <c r="B8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
+        <v>28</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="D8">
         <v>6584</v>
       </c>
+      <c r="F8" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="3"/>
       <c r="B9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
+        <v>29</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="D9">
         <v>6866</v>
       </c>
+      <c r="F9" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="A10" s="3"/>
       <c r="B10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" t="s">
-        <v>8</v>
+        <v>30</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="D10">
         <v>6859</v>
       </c>
+      <c r="F10" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="3"/>
       <c r="B11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
+        <v>31</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="D11">
         <v>6863</v>
       </c>
+      <c r="F11" s="1" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="3"/>
       <c r="B12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D12">
         <v>6865</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="F12" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
       <c r="B13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" t="s">
-        <v>15</v>
+        <v>33</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="D13">
         <v>6763</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+      <c r="A14" s="3"/>
       <c r="B14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D14">
         <v>6772</v>
       </c>
+      <c r="F14" s="1" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="3"/>
       <c r="B15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D15">
         <v>6851</v>
       </c>
+      <c r="F15" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="3"/>
       <c r="B16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D16">
@@ -790,116 +866,113 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="3"/>
       <c r="B17" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" t="s">
-        <v>18</v>
+        <v>36</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="D17">
         <v>6621</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+      <c r="A18" s="3"/>
       <c r="B18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" t="s">
-        <v>8</v>
+        <v>37</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="D18">
         <v>6834</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="A19" s="3"/>
       <c r="B19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" t="s">
-        <v>21</v>
+        <v>15</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="D19">
         <v>6973</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
       <c r="B20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" t="s">
-        <v>24</v>
+        <v>17</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="D20">
         <v>6628</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
       <c r="B21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" t="s">
-        <v>25</v>
+        <v>18</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="D21">
         <v>6629</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="3" t="s">
+      <c r="A22" s="3" t="s">
         <v>46</v>
       </c>
+      <c r="B22" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="C22" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D22">
         <v>6776</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
+      <c r="A23" s="3"/>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D23">
         <v>6776</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
+      <c r="A24" s="3"/>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C24" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D24">
         <v>6817</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
+      <c r="A25" s="3"/>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C25" t="s">
         <v>8</v>
@@ -909,9 +982,9 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
+      <c r="A26" s="3"/>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C26" t="s">
         <v>8</v>
@@ -921,53 +994,53 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>56</v>
+      <c r="A27" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="C27" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D27">
         <v>6709</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
+      <c r="A28" s="3"/>
       <c r="B28" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C28" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D28">
         <v>6709</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
+      <c r="A29" s="3"/>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C29" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D29">
         <v>6848</v>
       </c>
       <c r="F29" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" t="s">
-        <v>61</v>
       </c>
       <c r="C30" t="s">
         <v>8</v>
@@ -977,30 +1050,30 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
+      <c r="A31" s="3"/>
       <c r="B31" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C31" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D31">
         <v>6746</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
+      <c r="A32" s="3"/>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C32" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D32">
         <v>6758</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>